<commit_message>
manga v(2.12.0.1) Fix Reading Recorded Data
Server Side:
  - Fix coding bugs in Exam Loader's classes, now it can be extended to any other file types.
  - Fix the reading of Timing data from file, now it can detect the total spend time and
    appended to the student so that he can connect again after finish.
  - add feature of disconnected status.
  - add feature of Ungrade student and Unfinish him.
  - GUI: change IP and port to be in one label

Client Side:
  - GUI: change the style of quesion list navigator.

Gradle Side:-
  -

 Problem NOT SOLVED YET:
  - we need to move the validation method to be inside Student class
  - why the heap memory is keep increasing on each backup?
  - let the multiple choices boxes to be hidden without taking palce.
  - change exam time
  - ODS file loader still not implemented 100%
</commit_message>
<xml_diff>
--- a/data/MidTerm-1/SE260-MidTerm-1.xlsx
+++ b/data/MidTerm-1/SE260-MidTerm-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Sami-Programming\JAVA\eQuiz\data\MidTerm-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3040E83-3DDE-40B0-808A-1D03EB0E1871}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9921CCEB-C4C9-4DAF-8E47-5D5A0BFF4578}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10400" tabRatio="426" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12432" tabRatio="426" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="451">
   <si>
     <t>sharing folder</t>
   </si>
@@ -1465,6 +1465,9 @@
   </si>
   <si>
     <t>1:01:48</t>
+  </si>
+  <si>
+    <t>15.jpg</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1725,6 +1728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2228,8 +2232,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2245,19 +2249,19 @@
   <sheetData>
     <row r="1" spans="1:12" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -2323,7 +2327,9 @@
         <v>43</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="32"/>
+      <c r="J3" s="32" t="s">
+        <v>450</v>
+      </c>
       <c r="K3" s="14">
         <v>1</v>
       </c>
@@ -2876,7 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
@@ -4284,13 +4290,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="20" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4417,7 +4428,7 @@
       <c r="S2" t="s">
         <v>309</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="34" t="s">
         <v>310</v>
       </c>
       <c r="U2" t="s">
@@ -4482,7 +4493,7 @@
       <c r="S3" t="s">
         <v>326</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="34" t="s">
         <v>327</v>
       </c>
       <c r="U3" t="s">
@@ -4547,7 +4558,7 @@
       <c r="S4" t="s">
         <v>342</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="34" t="s">
         <v>343</v>
       </c>
       <c r="U4" t="s">
@@ -4612,7 +4623,7 @@
       <c r="S5" t="s">
         <v>357</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="34" t="s">
         <v>306</v>
       </c>
       <c r="U5" t="s">
@@ -4677,7 +4688,7 @@
       <c r="S6" t="s">
         <v>372</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="34" t="s">
         <v>373</v>
       </c>
       <c r="U6" t="s">
@@ -4742,7 +4753,7 @@
       <c r="S7" t="s">
         <v>389</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="34" t="s">
         <v>390</v>
       </c>
       <c r="U7" t="s">
@@ -4807,7 +4818,7 @@
       <c r="S8" t="s">
         <v>369</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="34" t="s">
         <v>403</v>
       </c>
       <c r="U8" t="s">
@@ -4872,7 +4883,7 @@
       <c r="S9" t="s">
         <v>415</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="34" t="s">
         <v>416</v>
       </c>
       <c r="U9" t="s">
@@ -4937,7 +4948,7 @@
       <c r="S10" t="s">
         <v>368</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="34" t="s">
         <v>426</v>
       </c>
       <c r="U10" t="s">
@@ -5002,7 +5013,7 @@
       <c r="S11" t="s">
         <v>438</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="34" t="s">
         <v>439</v>
       </c>
       <c r="U11" t="s">
@@ -5011,5 +5022,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
manga v(3.4.0.1)  Another update
Server Side:
  - Add Help Window
  - fix: correction icons beeing replaced with good ones.
  - fix: PDF exporter, now Question number and correct icons is added.
  - fix: some bugs in grading sheet
  - fix: grading sheet can be opened by double click.

Client Side:
  - can exploite the whole space of multiple choices.
  - Add Help Window
  - change icon of zoom.png

Core Side:
  - fix: now a config file is been made for saving any property
  - fix: shared images are moved to core resources folder.
  - fix: correct all questions code embedded in Student class.

Gradle Side:-

Problems NOT SOLVED YET:
  - add menu icons.
  - fix: let server can open any excel file immeaidatly.
  - complete JRE packaging using Java9 for both client and server.
  - can correct each student in GUI interface.
  - we need to move the validation method to be inside Student class.
  - ODS file loader still only 50% is implemented.
</commit_message>
<xml_diff>
--- a/data/MidTerm-1/SE260-MidTerm-1.xlsx
+++ b/data/MidTerm-1/SE260-MidTerm-1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Sami-Programming\JAVA\eQuiz\data\MidTerm-1\"/>
     </mc:Choice>
@@ -16,8 +16,9 @@
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
     <sheet name="BlackWhite_List" sheetId="3" r:id="rId3"/>
-    <sheet name="Answers" sheetId="4" r:id="rId4"/>
-    <sheet name="Timer" sheetId="5" r:id="rId5"/>
+    <sheet name="Answers" r:id="rId9" sheetId="6"/>
+    <sheet name="Timer" r:id="rId10" sheetId="7"/>
+    <sheet name="Log" r:id="rId11" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="496">
   <si>
     <t>sharing folder</t>
   </si>
@@ -1465,6 +1466,167 @@
   <si>
     <t>Q3`1`In a computer system, system resources are the components that provide its inherent capabilities and contribute to its overall performance.ex:cache memory
 In an operating system, system resources are internal tables and pointers set up to keep track of running applications.`not really</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>Q3`1`In a computer system, system resources are the components that provide its inherent capabilities and contribute to its overall performance.ex:cache memory
+In an operating system, system resources are internal tables and pointers set up to keep track of running applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q11`2`Programs are simply UI and GUI to system calls. Ex:File management 
+e.g windows explorer, open/save window.Ex:Programming-language support.
+Compilers, assemblers, debuggers
+</t>
+  </si>
+  <si>
+    <t>Q14`2`Computer system can be divided into 4 components:
+Hardware:
+CPU, memory, I/O devices
+Operating system:
+Controls and coordinates use of hardware among various applications and users
+Application programs – define the ways in which to solve the computing problems of the users
+Word processors, web browsers, video games
+Users:
+People, machines, other computers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q18`2`
+1)Caching: is data in use copied from slower to faster storage temporarily.
+2)Secondary-Storage Management	
+</t>
+  </si>
+  <si>
+    <t>Q4`1`Bootstrap program is loaded at power-up the PC.
+Loads OS kernel and starts execution</t>
+  </si>
+  <si>
+    <t>Q11`2`Communications 
+Status information</t>
+  </si>
+  <si>
+    <t>Q11`2`UI and GUI to system calls 
+windows expolare 
+open/ save windows</t>
+  </si>
+  <si>
+    <t>Q14`2`Process needs resources to accomplish its task
+CPU, memory, I/O, files, etc.
+Initialization data
+Process termination requires reclaim of any reusable resources.
+A thread is a basic unit of  CPU utilization within a process.</t>
+  </si>
+  <si>
+    <t>59:51</t>
+  </si>
+  <si>
+    <t>1:04:30</t>
+  </si>
+  <si>
+    <t>56:18</t>
+  </si>
+  <si>
+    <t>57:59</t>
+  </si>
+  <si>
+    <t>1:00:01</t>
+  </si>
+  <si>
+    <t>1:01:35</t>
+  </si>
+  <si>
+    <t>1:00:11</t>
+  </si>
+  <si>
+    <t>1:04:17</t>
+  </si>
+  <si>
+    <t>1:01:41</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:35:21</t>
+  </si>
+  <si>
+    <t>Server is Initialized, 192.168.200.1:10000</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:35:51</t>
+  </si>
+  <si>
+    <t>New Client has been joined, socketID = 1</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:36:58</t>
+  </si>
+  <si>
+    <t>Sending...</t>
+  </si>
+  <si>
+    <t>Exam Sheets are sent to 'Ready' and 'Resume' Students</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:37:03</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:37:22</t>
+  </si>
+  <si>
+    <t>New Client has been joined, socketID = 2</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:37:31</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:38:24</t>
+  </si>
+  <si>
+    <t>braa is Cut-Off his exam</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:38:44</t>
+  </si>
+  <si>
+    <t>New Client has been joined, socketID = 3</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:40:06</t>
+  </si>
+  <si>
+    <t>brad is Cut-Off his exam</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:45:13</t>
+  </si>
+  <si>
+    <t>New Client has been joined, socketID = 4</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:45:24</t>
+  </si>
+  <si>
+    <t>dasd is Cut-Off his exam</t>
+  </si>
+  <si>
+    <t>15-08-2019 04:45:36</t>
+  </si>
+  <si>
+    <t>Finishing...</t>
+  </si>
+  <si>
+    <t>All Students are alerted to Finish now!</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1785,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2080,9 +2244,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="50.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2238,13 +2402,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="9" width="8.81640625" style="7" collapsed="1"/>
-    <col min="10" max="10" width="12.81640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.81640625" style="5" collapsed="1"/>
-    <col min="12" max="12" width="10" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="3.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="9" style="7" width="8.81640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="7" width="12.81640625" collapsed="true"/>
+    <col min="11" max="11" style="5" width="8.81640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="5" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2852,8 +3016,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="16.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="2" width="8.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="16.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2878,58 +3042,56 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6328125" customWidth="1"/>
-    <col min="9" max="9" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.6328125" customWidth="1"/>
-    <col min="11" max="11" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="50.6328125" customWidth="1"/>
-    <col min="13" max="13" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="50.6328125" customWidth="1"/>
-    <col min="25" max="25" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="50.6328125" customWidth="1"/>
-    <col min="31" max="31" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="50.6328125" customWidth="1"/>
-    <col min="37" max="37" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="50.6328125" customWidth="1"/>
-    <col min="39" max="39" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.3046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="48.9296875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.01171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="213.58203125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="11.58203125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="13.015625" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="10.41015625" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="11.58203125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="14.1328125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="12.69921875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="11.5234375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="11.5234375" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.69921875" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="191.5390625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="3.8203125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="204.08203125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="3.8203125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2943,115 +3105,115 @@
         <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="F1" t="s">
         <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="H1" t="s">
         <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="J1" t="s">
         <v>102</v>
       </c>
       <c r="K1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="L1" t="s">
         <v>103</v>
       </c>
       <c r="M1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="N1" t="s">
         <v>104</v>
       </c>
       <c r="O1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="P1" t="s">
         <v>105</v>
       </c>
       <c r="Q1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="R1" t="s">
         <v>106</v>
       </c>
       <c r="S1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="T1" t="s">
         <v>107</v>
       </c>
       <c r="U1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="V1" t="s">
         <v>108</v>
       </c>
       <c r="W1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="X1" t="s">
         <v>109</v>
       </c>
       <c r="Y1" t="s">
-        <v>99</v>
+        <v>451</v>
       </c>
       <c r="Z1" t="s">
         <v>110</v>
       </c>
       <c r="AA1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="AB1" t="s">
         <v>111</v>
       </c>
       <c r="AC1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="AD1" t="s">
         <v>112</v>
       </c>
       <c r="AE1" t="s">
-        <v>99</v>
+        <v>451</v>
       </c>
       <c r="AF1" t="s">
         <v>113</v>
       </c>
       <c r="AG1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="AH1" t="s">
         <v>114</v>
       </c>
       <c r="AI1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="AJ1" t="s">
         <v>115</v>
       </c>
       <c r="AK1" t="s">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="AL1" t="s">
         <v>116</v>
       </c>
       <c r="AM1" t="s">
-        <v>99</v>
+        <v>451</v>
       </c>
       <c r="AN1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -3064,122 +3226,122 @@
       <c r="D2" t="s">
         <v>120</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="n">
+        <v>1.0</v>
       </c>
       <c r="F2" t="s">
         <v>121</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="n">
+        <v>1.0</v>
       </c>
       <c r="H2" t="s">
         <v>122</v>
       </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="n">
+        <v>1.0</v>
       </c>
       <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="K2">
-        <v>1</v>
+      <c r="K2" t="n">
+        <v>1.0</v>
       </c>
       <c r="L2" t="s">
         <v>124</v>
       </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="M2" t="n">
+        <v>1.0</v>
       </c>
       <c r="N2" t="s">
         <v>447</v>
       </c>
-      <c r="O2">
-        <v>1</v>
+      <c r="O2" t="n">
+        <v>1.0</v>
       </c>
       <c r="P2" t="s">
         <v>125</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
+      <c r="Q2" t="n">
+        <v>1.0</v>
       </c>
       <c r="R2" t="s">
         <v>126</v>
       </c>
-      <c r="S2">
-        <v>1</v>
+      <c r="S2" t="n">
+        <v>1.0</v>
       </c>
       <c r="T2" t="s">
         <v>127</v>
       </c>
-      <c r="U2">
-        <v>0</v>
+      <c r="U2" t="n">
+        <v>0.0</v>
       </c>
       <c r="V2" t="s">
         <v>128</v>
       </c>
-      <c r="W2">
-        <v>1</v>
+      <c r="W2" t="n">
+        <v>1.0</v>
       </c>
       <c r="X2" t="s">
         <v>129</v>
       </c>
-      <c r="Y2">
-        <v>0</v>
+      <c r="Y2" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z2" t="s">
         <v>446</v>
       </c>
-      <c r="AA2">
-        <v>1</v>
+      <c r="AA2" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB2" t="s">
         <v>149</v>
       </c>
-      <c r="AC2">
-        <v>1</v>
+      <c r="AC2" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD2" t="s">
         <v>130</v>
       </c>
-      <c r="AE2">
-        <v>2</v>
+      <c r="AE2" t="n">
+        <v>2.0</v>
       </c>
       <c r="AF2" t="s">
         <v>168</v>
       </c>
-      <c r="AG2">
-        <v>1</v>
+      <c r="AG2" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH2" t="s">
         <v>132</v>
       </c>
-      <c r="AI2">
-        <v>1</v>
+      <c r="AI2" t="n">
+        <v>1.0</v>
       </c>
       <c r="AJ2" t="s">
         <v>133</v>
       </c>
-      <c r="AK2">
-        <v>1</v>
+      <c r="AK2" t="n">
+        <v>1.0</v>
       </c>
       <c r="AL2" t="s">
         <v>134</v>
       </c>
-      <c r="AM2">
-        <v>2</v>
-      </c>
-      <c r="AN2">
-        <f t="shared" ref="AN2:AN11" si="0">SUMIF(D2:AM2,  "&gt;0")</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="AM2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN2" t="n">
+        <f> SUMIF(D2:AM2 ,  "&gt;0") </f>
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>452</v>
       </c>
       <c r="C3" t="s">
         <v>137</v>
@@ -3187,117 +3349,117 @@
       <c r="D3" t="s">
         <v>138</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" t="n">
+        <v>1.0</v>
       </c>
       <c r="F3" t="s">
         <v>139</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>449</v>
-      </c>
-      <c r="I3">
+      <c r="G3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>453</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.5</v>
       </c>
       <c r="J3" t="s">
         <v>140</v>
       </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="K3" t="n">
+        <v>0.0</v>
       </c>
       <c r="L3" t="s">
         <v>141</v>
       </c>
-      <c r="M3">
-        <v>0</v>
+      <c r="M3" t="n">
+        <v>0.0</v>
       </c>
       <c r="N3" t="s">
         <v>142</v>
       </c>
-      <c r="O3">
-        <v>0</v>
+      <c r="O3" t="n">
+        <v>0.0</v>
       </c>
       <c r="P3" t="s">
         <v>143</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
+      <c r="Q3" t="n">
+        <v>1.0</v>
       </c>
       <c r="R3" t="s">
         <v>144</v>
       </c>
-      <c r="S3">
-        <v>1</v>
+      <c r="S3" t="n">
+        <v>1.0</v>
       </c>
       <c r="T3" t="s">
         <v>145</v>
       </c>
-      <c r="U3">
-        <v>1</v>
+      <c r="U3" t="n">
+        <v>1.0</v>
       </c>
       <c r="V3" t="s">
         <v>146</v>
       </c>
-      <c r="W3">
-        <v>1</v>
+      <c r="W3" t="n">
+        <v>1.0</v>
       </c>
       <c r="X3" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y3">
-        <v>1</v>
+        <v>454</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1.0</v>
       </c>
       <c r="Z3" t="s">
         <v>148</v>
       </c>
-      <c r="AA3">
-        <v>1</v>
+      <c r="AA3" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB3" t="s">
         <v>149</v>
       </c>
-      <c r="AC3">
-        <v>1</v>
+      <c r="AC3" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
+        <v>455</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF3" t="s">
         <v>131</v>
       </c>
-      <c r="AG3">
-        <v>0</v>
+      <c r="AG3" t="n">
+        <v>0.0</v>
       </c>
       <c r="AH3" t="s">
         <v>151</v>
       </c>
-      <c r="AI3">
-        <v>0</v>
+      <c r="AI3" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ3" t="s">
         <v>152</v>
       </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="36" t="s">
-        <v>448</v>
-      </c>
-      <c r="AM3">
-        <v>1</v>
-      </c>
-      <c r="AN3">
-        <f t="shared" si="0"/>
+      <c r="AK3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>456</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AN3" t="n">
+        <f> SUMIF(D3:AM3 ,  "&gt;0") </f>
         <v>10.5</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -3310,117 +3472,117 @@
       <c r="D4" t="s">
         <v>156</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="n">
+        <v>1.0</v>
       </c>
       <c r="F4" t="s">
         <v>121</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="G4" t="n">
+        <v>1.0</v>
       </c>
       <c r="H4" t="s">
         <v>157</v>
       </c>
-      <c r="I4">
-        <v>0</v>
+      <c r="I4" t="n">
+        <v>0.0</v>
       </c>
       <c r="J4" t="s">
         <v>158</v>
       </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="K4" t="n">
+        <v>0.0</v>
       </c>
       <c r="L4" t="s">
         <v>159</v>
       </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="M4" t="n">
+        <v>0.0</v>
       </c>
       <c r="N4" t="s">
         <v>160</v>
       </c>
-      <c r="O4">
-        <v>0</v>
+      <c r="O4" t="n">
+        <v>0.0</v>
       </c>
       <c r="P4" t="s">
         <v>161</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
+      <c r="Q4" t="n">
+        <v>1.0</v>
       </c>
       <c r="R4" t="s">
         <v>126</v>
       </c>
-      <c r="S4">
-        <v>1</v>
+      <c r="S4" t="n">
+        <v>1.0</v>
       </c>
       <c r="T4" t="s">
         <v>162</v>
       </c>
-      <c r="U4">
-        <v>0</v>
+      <c r="U4" t="n">
+        <v>0.0</v>
       </c>
       <c r="V4" t="s">
         <v>163</v>
       </c>
-      <c r="W4">
-        <v>1</v>
+      <c r="W4" t="n">
+        <v>1.0</v>
       </c>
       <c r="X4" t="s">
         <v>164</v>
       </c>
-      <c r="Y4">
-        <v>0</v>
+      <c r="Y4" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z4" t="s">
         <v>165</v>
       </c>
-      <c r="AA4">
-        <v>1</v>
+      <c r="AA4" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB4" t="s">
         <v>166</v>
       </c>
-      <c r="AC4">
-        <v>1</v>
+      <c r="AC4" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD4" t="s">
         <v>167</v>
       </c>
-      <c r="AE4">
-        <v>0</v>
+      <c r="AE4" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF4" t="s">
         <v>168</v>
       </c>
-      <c r="AG4">
-        <v>1</v>
+      <c r="AG4" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH4" t="s">
         <v>169</v>
       </c>
-      <c r="AI4">
-        <v>0</v>
+      <c r="AI4" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ4" t="s">
         <v>170</v>
       </c>
-      <c r="AK4">
-        <v>1</v>
+      <c r="AK4" t="n">
+        <v>1.0</v>
       </c>
       <c r="AL4" t="s">
         <v>171</v>
       </c>
-      <c r="AM4">
-        <v>2</v>
-      </c>
-      <c r="AN4">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN4" t="n">
+        <f> SUMIF(D4:AM4 ,  "&gt;0") </f>
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -3433,117 +3595,117 @@
       <c r="D5" t="s">
         <v>175</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" t="n">
+        <v>0.0</v>
       </c>
       <c r="F5" t="s">
         <v>176</v>
       </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="G5" t="n">
+        <v>0.0</v>
       </c>
       <c r="H5" t="s">
         <v>177</v>
       </c>
-      <c r="I5">
-        <v>0</v>
+      <c r="I5" t="n">
+        <v>0.0</v>
       </c>
       <c r="J5" t="s">
-        <v>178</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
+        <v>457</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0</v>
       </c>
       <c r="L5" t="s">
         <v>179</v>
       </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="M5" t="n">
+        <v>0.0</v>
       </c>
       <c r="N5" t="s">
         <v>180</v>
       </c>
-      <c r="O5">
-        <v>0</v>
+      <c r="O5" t="n">
+        <v>0.0</v>
       </c>
       <c r="P5" t="s">
         <v>181</v>
       </c>
-      <c r="Q5">
-        <v>1</v>
+      <c r="Q5" t="n">
+        <v>1.0</v>
       </c>
       <c r="R5" t="s">
         <v>126</v>
       </c>
-      <c r="S5">
-        <v>1</v>
+      <c r="S5" t="n">
+        <v>1.0</v>
       </c>
       <c r="T5" t="s">
         <v>182</v>
       </c>
-      <c r="U5">
-        <v>0</v>
+      <c r="U5" t="n">
+        <v>0.0</v>
       </c>
       <c r="V5" t="s">
         <v>183</v>
       </c>
-      <c r="W5">
-        <v>1</v>
+      <c r="W5" t="n">
+        <v>1.0</v>
       </c>
       <c r="X5" t="s">
         <v>184</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
+      <c r="Y5" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z5" t="s">
         <v>148</v>
       </c>
-      <c r="AA5">
-        <v>1</v>
+      <c r="AA5" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB5" t="s">
         <v>149</v>
       </c>
-      <c r="AC5">
-        <v>1</v>
+      <c r="AC5" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD5" t="s">
         <v>185</v>
       </c>
-      <c r="AE5">
-        <v>0</v>
+      <c r="AE5" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF5" t="s">
         <v>168</v>
       </c>
-      <c r="AG5">
-        <v>1</v>
+      <c r="AG5" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH5" t="s">
         <v>186</v>
       </c>
-      <c r="AI5">
-        <v>0</v>
+      <c r="AI5" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ5" t="s">
         <v>187</v>
       </c>
-      <c r="AK5">
-        <v>1</v>
+      <c r="AK5" t="n">
+        <v>1.0</v>
       </c>
       <c r="AL5" t="s">
         <v>188</v>
       </c>
-      <c r="AM5">
-        <v>0</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN5" t="n">
+        <f> SUMIF(D5:AM5 ,  "&gt;0") </f>
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -3556,117 +3718,117 @@
       <c r="D6" t="s">
         <v>192</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" t="n">
+        <v>0.0</v>
       </c>
       <c r="F6" t="s">
         <v>193</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" t="n">
+        <v>0.0</v>
       </c>
       <c r="H6" t="s">
         <v>194</v>
       </c>
-      <c r="I6">
-        <v>0</v>
+      <c r="I6" t="n">
+        <v>0.0</v>
       </c>
       <c r="J6" t="s">
         <v>195</v>
       </c>
-      <c r="K6">
-        <v>0</v>
+      <c r="K6" t="n">
+        <v>0.0</v>
       </c>
       <c r="L6" t="s">
         <v>196</v>
       </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="M6" t="n">
+        <v>0.0</v>
       </c>
       <c r="N6" t="s">
         <v>197</v>
       </c>
-      <c r="O6">
-        <v>1</v>
+      <c r="O6" t="n">
+        <v>1.0</v>
       </c>
       <c r="P6" t="s">
         <v>198</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
+      <c r="Q6" t="n">
+        <v>1.0</v>
       </c>
       <c r="R6" t="s">
         <v>199</v>
       </c>
-      <c r="S6">
-        <v>0</v>
+      <c r="S6" t="n">
+        <v>0.0</v>
       </c>
       <c r="T6" t="s">
         <v>127</v>
       </c>
-      <c r="U6">
-        <v>0</v>
+      <c r="U6" t="n">
+        <v>0.0</v>
       </c>
       <c r="V6" t="s">
         <v>200</v>
       </c>
-      <c r="W6">
-        <v>1</v>
+      <c r="W6" t="n">
+        <v>1.0</v>
       </c>
       <c r="X6" t="s">
         <v>201</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
+      <c r="Y6" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z6" t="s">
         <v>202</v>
       </c>
-      <c r="AA6">
-        <v>0</v>
+      <c r="AA6" t="n">
+        <v>0.0</v>
       </c>
       <c r="AB6" t="s">
         <v>149</v>
       </c>
-      <c r="AC6">
-        <v>1</v>
+      <c r="AC6" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD6" t="s">
         <v>185</v>
       </c>
-      <c r="AE6">
-        <v>0</v>
+      <c r="AE6" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF6" t="s">
         <v>203</v>
       </c>
-      <c r="AG6">
-        <v>1</v>
+      <c r="AG6" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH6" t="s">
         <v>169</v>
       </c>
-      <c r="AI6">
-        <v>0</v>
+      <c r="AI6" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ6" t="s">
         <v>204</v>
       </c>
-      <c r="AK6">
-        <v>0</v>
+      <c r="AK6" t="n">
+        <v>0.0</v>
       </c>
       <c r="AL6" t="s">
         <v>205</v>
       </c>
-      <c r="AM6">
-        <v>2</v>
-      </c>
-      <c r="AN6">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN6" t="n">
+        <f> SUMIF(D6:AM6 ,  "&gt;0") </f>
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -3679,117 +3841,117 @@
       <c r="D7" t="s">
         <v>209</v>
       </c>
-      <c r="E7">
-        <v>0</v>
+      <c r="E7" t="n">
+        <v>0.0</v>
       </c>
       <c r="F7" t="s">
         <v>210</v>
       </c>
-      <c r="G7">
-        <v>1</v>
+      <c r="G7" t="n">
+        <v>1.0</v>
       </c>
       <c r="H7" t="s">
         <v>211</v>
       </c>
-      <c r="I7">
-        <v>0</v>
+      <c r="I7" t="n">
+        <v>0.0</v>
       </c>
       <c r="J7" t="s">
         <v>212</v>
       </c>
-      <c r="K7">
-        <v>0</v>
+      <c r="K7" t="n">
+        <v>0.0</v>
       </c>
       <c r="L7" t="s">
         <v>213</v>
       </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="M7" t="n">
+        <v>0.0</v>
       </c>
       <c r="N7" t="s">
         <v>214</v>
       </c>
-      <c r="O7">
-        <v>0</v>
+      <c r="O7" t="n">
+        <v>0.0</v>
       </c>
       <c r="P7" t="s">
         <v>215</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
+      <c r="Q7" t="n">
+        <v>0.0</v>
       </c>
       <c r="R7" t="s">
         <v>126</v>
       </c>
-      <c r="S7">
-        <v>1</v>
+      <c r="S7" t="n">
+        <v>1.0</v>
       </c>
       <c r="T7" t="s">
         <v>216</v>
       </c>
-      <c r="U7">
-        <v>1</v>
+      <c r="U7" t="n">
+        <v>1.0</v>
       </c>
       <c r="V7" t="s">
         <v>217</v>
       </c>
-      <c r="W7">
-        <v>0</v>
+      <c r="W7" t="n">
+        <v>0.0</v>
       </c>
       <c r="X7" t="s">
         <v>218</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
+      <c r="Y7" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z7" t="s">
         <v>219</v>
       </c>
-      <c r="AA7">
-        <v>1</v>
+      <c r="AA7" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB7" t="s">
         <v>166</v>
       </c>
-      <c r="AC7">
-        <v>1</v>
+      <c r="AC7" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD7" t="s">
         <v>220</v>
       </c>
-      <c r="AE7">
-        <v>0</v>
+      <c r="AE7" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF7" t="s">
         <v>203</v>
       </c>
-      <c r="AG7">
-        <v>1</v>
+      <c r="AG7" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH7" t="s">
         <v>221</v>
       </c>
-      <c r="AI7">
-        <v>1</v>
+      <c r="AI7" t="n">
+        <v>1.0</v>
       </c>
       <c r="AJ7" t="s">
         <v>222</v>
       </c>
-      <c r="AK7">
-        <v>0</v>
+      <c r="AK7" t="n">
+        <v>0.0</v>
       </c>
       <c r="AL7" t="s">
         <v>223</v>
       </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN7" t="n">
+        <f> SUMIF(D7:AM7 ,  "&gt;0") </f>
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3802,117 +3964,117 @@
       <c r="D8" t="s">
         <v>227</v>
       </c>
-      <c r="E8">
-        <v>1</v>
+      <c r="E8" t="n">
+        <v>1.0</v>
       </c>
       <c r="F8" t="s">
         <v>228</v>
       </c>
-      <c r="G8">
-        <v>1</v>
+      <c r="G8" t="n">
+        <v>1.0</v>
       </c>
       <c r="H8" t="s">
         <v>229</v>
       </c>
-      <c r="I8">
-        <v>0</v>
+      <c r="I8" t="n">
+        <v>0.0</v>
       </c>
       <c r="J8" t="s">
         <v>230</v>
       </c>
-      <c r="K8">
-        <v>0</v>
+      <c r="K8" t="n">
+        <v>0.0</v>
       </c>
       <c r="L8" t="s">
         <v>231</v>
       </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="M8" t="n">
+        <v>0.0</v>
       </c>
       <c r="N8" t="s">
         <v>232</v>
       </c>
-      <c r="O8">
-        <v>1</v>
+      <c r="O8" t="n">
+        <v>1.0</v>
       </c>
       <c r="P8" t="s">
         <v>233</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
+      <c r="Q8" t="n">
+        <v>1.0</v>
       </c>
       <c r="R8" t="s">
         <v>144</v>
       </c>
-      <c r="S8">
-        <v>1</v>
+      <c r="S8" t="n">
+        <v>1.0</v>
       </c>
       <c r="T8" t="s">
         <v>234</v>
       </c>
-      <c r="U8">
-        <v>0</v>
+      <c r="U8" t="n">
+        <v>0.0</v>
       </c>
       <c r="V8" t="s">
         <v>235</v>
       </c>
-      <c r="W8">
-        <v>0</v>
+      <c r="W8" t="n">
+        <v>0.0</v>
       </c>
       <c r="X8" t="s">
-        <v>236</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
+        <v>458</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z8" t="s">
         <v>237</v>
       </c>
-      <c r="AA8">
-        <v>0</v>
+      <c r="AA8" t="n">
+        <v>0.0</v>
       </c>
       <c r="AB8" t="s">
         <v>149</v>
       </c>
-      <c r="AC8">
-        <v>1</v>
+      <c r="AC8" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD8" t="s">
         <v>238</v>
       </c>
-      <c r="AE8">
-        <v>0</v>
+      <c r="AE8" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF8" t="s">
         <v>239</v>
       </c>
-      <c r="AG8">
-        <v>0</v>
+      <c r="AG8" t="n">
+        <v>0.0</v>
       </c>
       <c r="AH8" t="s">
         <v>151</v>
       </c>
-      <c r="AI8">
-        <v>0</v>
+      <c r="AI8" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ8" t="s">
         <v>240</v>
       </c>
-      <c r="AK8">
-        <v>0</v>
+      <c r="AK8" t="n">
+        <v>0.0</v>
       </c>
       <c r="AL8" t="s">
         <v>241</v>
       </c>
-      <c r="AM8">
-        <v>0</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN8" t="n">
+        <f> SUMIF(D8:AM8 ,  "&gt;0") </f>
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -3925,117 +4087,117 @@
       <c r="D9" t="s">
         <v>245</v>
       </c>
-      <c r="E9">
-        <v>1</v>
+      <c r="E9" t="n">
+        <v>1.0</v>
       </c>
       <c r="F9" t="s">
         <v>246</v>
       </c>
-      <c r="G9">
-        <v>1</v>
+      <c r="G9" t="n">
+        <v>1.0</v>
       </c>
       <c r="H9" t="s">
         <v>247</v>
       </c>
-      <c r="I9">
-        <v>0</v>
+      <c r="I9" t="n">
+        <v>0.0</v>
       </c>
       <c r="J9" t="s">
         <v>248</v>
       </c>
-      <c r="K9">
-        <v>0</v>
+      <c r="K9" t="n">
+        <v>0.0</v>
       </c>
       <c r="L9" t="s">
         <v>249</v>
       </c>
-      <c r="M9">
-        <v>0</v>
+      <c r="M9" t="n">
+        <v>0.0</v>
       </c>
       <c r="N9" t="s">
         <v>232</v>
       </c>
-      <c r="O9">
-        <v>1</v>
+      <c r="O9" t="n">
+        <v>1.0</v>
       </c>
       <c r="P9" t="s">
         <v>250</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
+      <c r="Q9" t="n">
+        <v>1.0</v>
       </c>
       <c r="R9" t="s">
         <v>126</v>
       </c>
-      <c r="S9">
-        <v>1</v>
+      <c r="S9" t="n">
+        <v>1.0</v>
       </c>
       <c r="T9" t="s">
         <v>251</v>
       </c>
-      <c r="U9">
-        <v>1</v>
+      <c r="U9" t="n">
+        <v>1.0</v>
       </c>
       <c r="V9" t="s">
         <v>252</v>
       </c>
-      <c r="W9">
-        <v>1</v>
+      <c r="W9" t="n">
+        <v>1.0</v>
       </c>
       <c r="X9" t="s">
         <v>253</v>
       </c>
-      <c r="Y9">
-        <v>0</v>
+      <c r="Y9" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z9" t="s">
         <v>254</v>
       </c>
-      <c r="AA9">
-        <v>1</v>
+      <c r="AA9" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB9" t="s">
         <v>149</v>
       </c>
-      <c r="AC9">
-        <v>1</v>
+      <c r="AC9" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD9" t="s">
         <v>255</v>
       </c>
-      <c r="AE9">
-        <v>0</v>
+      <c r="AE9" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF9" t="s">
         <v>131</v>
       </c>
-      <c r="AG9">
-        <v>0</v>
+      <c r="AG9" t="n">
+        <v>0.0</v>
       </c>
       <c r="AH9" t="s">
         <v>256</v>
       </c>
-      <c r="AI9">
-        <v>0</v>
+      <c r="AI9" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ9" t="s">
         <v>257</v>
       </c>
-      <c r="AK9">
-        <v>1</v>
+      <c r="AK9" t="n">
+        <v>1.0</v>
       </c>
       <c r="AL9" t="s">
         <v>258</v>
       </c>
-      <c r="AM9">
-        <v>2</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN9" t="n">
+        <f> SUMIF(D9:AM9 ,  "&gt;0") </f>
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -4048,117 +4210,117 @@
       <c r="D10" t="s">
         <v>262</v>
       </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="E10" t="n">
+        <v>0.0</v>
       </c>
       <c r="F10" t="s">
         <v>176</v>
       </c>
-      <c r="G10">
-        <v>0</v>
+      <c r="G10" t="n">
+        <v>0.0</v>
       </c>
       <c r="H10" t="s">
         <v>263</v>
       </c>
-      <c r="I10">
-        <v>0</v>
+      <c r="I10" t="n">
+        <v>0.0</v>
       </c>
       <c r="J10" t="s">
         <v>264</v>
       </c>
-      <c r="K10">
-        <v>0</v>
+      <c r="K10" t="n">
+        <v>0.0</v>
       </c>
       <c r="L10" t="s">
         <v>265</v>
       </c>
-      <c r="M10">
-        <v>0</v>
+      <c r="M10" t="n">
+        <v>0.0</v>
       </c>
       <c r="N10" t="s">
         <v>266</v>
       </c>
-      <c r="O10">
-        <v>0</v>
+      <c r="O10" t="n">
+        <v>0.0</v>
       </c>
       <c r="P10" t="s">
         <v>267</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
+      <c r="Q10" t="n">
+        <v>0.0</v>
       </c>
       <c r="R10" t="s">
         <v>144</v>
       </c>
-      <c r="S10">
-        <v>1</v>
+      <c r="S10" t="n">
+        <v>1.0</v>
       </c>
       <c r="T10" t="s">
         <v>268</v>
       </c>
-      <c r="U10">
-        <v>0</v>
+      <c r="U10" t="n">
+        <v>0.0</v>
       </c>
       <c r="V10" t="s">
         <v>269</v>
       </c>
-      <c r="W10">
-        <v>0</v>
+      <c r="W10" t="n">
+        <v>0.0</v>
       </c>
       <c r="X10" t="s">
         <v>270</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
+      <c r="Y10" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z10" t="s">
         <v>271</v>
       </c>
-      <c r="AA10">
-        <v>0</v>
+      <c r="AA10" t="n">
+        <v>0.0</v>
       </c>
       <c r="AB10" t="s">
         <v>149</v>
       </c>
-      <c r="AC10">
-        <v>1</v>
+      <c r="AC10" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD10" t="s">
         <v>272</v>
       </c>
-      <c r="AE10">
-        <v>0</v>
+      <c r="AE10" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF10" t="s">
         <v>203</v>
       </c>
-      <c r="AG10">
-        <v>1</v>
+      <c r="AG10" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH10" t="s">
         <v>221</v>
       </c>
-      <c r="AI10">
-        <v>1</v>
+      <c r="AI10" t="n">
+        <v>1.0</v>
       </c>
       <c r="AJ10" t="s">
         <v>273</v>
       </c>
-      <c r="AK10">
-        <v>0</v>
+      <c r="AK10" t="n">
+        <v>0.0</v>
       </c>
       <c r="AL10" t="s">
         <v>223</v>
       </c>
-      <c r="AM10">
-        <v>2</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AM10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN10" t="n">
+        <f> SUMIF(D10:AM10 ,  "&gt;0") </f>
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -4171,141 +4333,153 @@
       <c r="D11" t="s">
         <v>277</v>
       </c>
-      <c r="E11">
-        <v>1</v>
+      <c r="E11" t="n">
+        <v>1.0</v>
       </c>
       <c r="F11" t="s">
         <v>278</v>
       </c>
-      <c r="G11">
-        <v>0</v>
+      <c r="G11" t="n">
+        <v>0.0</v>
       </c>
       <c r="H11" t="s">
         <v>279</v>
       </c>
-      <c r="I11">
-        <v>0</v>
+      <c r="I11" t="n">
+        <v>0.0</v>
       </c>
       <c r="J11" t="s">
         <v>280</v>
       </c>
-      <c r="K11">
-        <v>0</v>
+      <c r="K11" t="n">
+        <v>0.0</v>
       </c>
       <c r="L11" t="s">
         <v>281</v>
       </c>
-      <c r="M11">
-        <v>0</v>
+      <c r="M11" t="n">
+        <v>0.0</v>
       </c>
       <c r="N11" t="s">
         <v>214</v>
       </c>
-      <c r="O11">
-        <v>0</v>
+      <c r="O11" t="n">
+        <v>0.0</v>
       </c>
       <c r="P11" t="s">
         <v>198</v>
       </c>
-      <c r="Q11">
-        <v>1</v>
+      <c r="Q11" t="n">
+        <v>1.0</v>
       </c>
       <c r="R11" t="s">
         <v>144</v>
       </c>
-      <c r="S11">
-        <v>1</v>
+      <c r="S11" t="n">
+        <v>1.0</v>
       </c>
       <c r="T11" t="s">
         <v>145</v>
       </c>
-      <c r="U11">
-        <v>1</v>
+      <c r="U11" t="n">
+        <v>1.0</v>
       </c>
       <c r="V11" t="s">
         <v>282</v>
       </c>
-      <c r="W11">
-        <v>0</v>
+      <c r="W11" t="n">
+        <v>0.0</v>
       </c>
       <c r="X11" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
+        <v>459</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.0</v>
       </c>
       <c r="Z11" t="s">
         <v>284</v>
       </c>
-      <c r="AA11">
-        <v>1</v>
+      <c r="AA11" t="n">
+        <v>1.0</v>
       </c>
       <c r="AB11" t="s">
         <v>166</v>
       </c>
-      <c r="AC11">
-        <v>1</v>
+      <c r="AC11" t="n">
+        <v>1.0</v>
       </c>
       <c r="AD11" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
+        <v>460</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.0</v>
       </c>
       <c r="AF11" t="s">
         <v>203</v>
       </c>
-      <c r="AG11">
-        <v>1</v>
+      <c r="AG11" t="n">
+        <v>1.0</v>
       </c>
       <c r="AH11" t="s">
         <v>286</v>
       </c>
-      <c r="AI11">
-        <v>0</v>
+      <c r="AI11" t="n">
+        <v>0.0</v>
       </c>
       <c r="AJ11" t="s">
         <v>287</v>
       </c>
-      <c r="AK11">
-        <v>1</v>
+      <c r="AK11" t="n">
+        <v>1.0</v>
       </c>
       <c r="AL11" t="s">
         <v>288</v>
       </c>
-      <c r="AM11">
-        <v>2</v>
-      </c>
-      <c r="AN11">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="AM11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AN11" t="n">
+        <f> SUMIF(D11:AM11 ,  "&gt;0") </f>
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="0.1953125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="0.1953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -4370,7 +4544,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -4428,19 +4602,19 @@
       <c r="S2" t="s">
         <v>304</v>
       </c>
-      <c r="T2" s="34" t="s">
+      <c r="T2" t="s">
         <v>305</v>
       </c>
       <c r="U2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>452</v>
       </c>
       <c r="C3" t="s">
         <v>306</v>
@@ -4493,14 +4667,14 @@
       <c r="S3" t="s">
         <v>321</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T3" t="s">
         <v>322</v>
       </c>
       <c r="U3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -4558,14 +4732,14 @@
       <c r="S4" t="s">
         <v>337</v>
       </c>
-      <c r="T4" s="34" t="s">
+      <c r="T4" t="s">
         <v>338</v>
       </c>
       <c r="U4" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -4623,14 +4797,14 @@
       <c r="S5" t="s">
         <v>352</v>
       </c>
-      <c r="T5" s="34" t="s">
+      <c r="T5" t="s">
         <v>301</v>
       </c>
       <c r="U5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -4688,14 +4862,14 @@
       <c r="S6" t="s">
         <v>367</v>
       </c>
-      <c r="T6" s="34" t="s">
+      <c r="T6" t="s">
         <v>368</v>
       </c>
       <c r="U6" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -4753,14 +4927,14 @@
       <c r="S7" t="s">
         <v>384</v>
       </c>
-      <c r="T7" s="34" t="s">
+      <c r="T7" t="s">
         <v>385</v>
       </c>
       <c r="U7" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -4818,14 +4992,14 @@
       <c r="S8" t="s">
         <v>364</v>
       </c>
-      <c r="T8" s="34" t="s">
+      <c r="T8" t="s">
         <v>398</v>
       </c>
       <c r="U8" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -4883,14 +5057,14 @@
       <c r="S9" t="s">
         <v>410</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" t="s">
         <v>411</v>
       </c>
       <c r="U9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -4948,14 +5122,14 @@
       <c r="S10" t="s">
         <v>363</v>
       </c>
-      <c r="T10" s="34" t="s">
+      <c r="T10" t="s">
         <v>421</v>
       </c>
       <c r="U10" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -5013,15 +5187,163 @@
       <c r="S11" t="s">
         <v>433</v>
       </c>
-      <c r="T11" s="34" t="s">
+      <c r="T11" t="s">
         <v>434</v>
       </c>
       <c r="U11" t="s">
-        <v>444</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>480</v>
+      </c>
+      <c r="B8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B9" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>482</v>
+      </c>
+      <c r="B10" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>483</v>
+      </c>
+      <c r="B11" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>485</v>
+      </c>
+      <c r="B12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>491</v>
+      </c>
+      <c r="B15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>493</v>
+      </c>
+      <c r="B16" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>493</v>
+      </c>
+      <c r="B17" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>